<commit_message>
Update LinearRegression 2 final.xlsx
Update
</commit_message>
<xml_diff>
--- a/LinearRegression 2 final.xlsx
+++ b/LinearRegression 2 final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Temperature (C)</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>sum of errors</t>
-  </si>
-  <si>
-    <t>Sunny Days</t>
   </si>
   <si>
     <t>Holidays</t>
@@ -389,7 +386,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>

</xml_diff>